<commit_message>
Further updates on staff and inventory manager
</commit_message>
<xml_diff>
--- a/data/MedicalInventory_List.xlsx
+++ b/data/MedicalInventory_List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Part Time Studies\OOP_Proj\data\"/>
     </mc:Choice>
@@ -659,6 +659,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1023,13 +1024,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="11.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="19.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="18.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="19.5703125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="17.5703125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="24.140625"/>
+    <col min="7" max="16384" style="2" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,14 +3043,14 @@
       <c r="C101" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D101" s="2">
-        <v>2</v>
+      <c r="D101" s="2" t="n">
+        <v>43.0</v>
       </c>
       <c r="E101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F101" s="2">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="F101" s="2" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inventory manager list refresh and print formatting
</commit_message>
<xml_diff>
--- a/data/MedicalInventory_List.xlsx
+++ b/data/MedicalInventory_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="214">
   <si>
     <t>MedicineID</t>
   </si>
@@ -653,6 +653,15 @@
   </si>
   <si>
     <t>Alendronate</t>
+  </si>
+  <si>
+    <t>M101</t>
+  </si>
+  <si>
+    <t>Fentanyl</t>
+  </si>
+  <si>
+    <t>Drugs lol</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixed Admin Bugs, Implemented Appoitment view for admin
</commit_message>
<xml_diff>
--- a/data/MedicalInventory_List.xlsx
+++ b/data/MedicalInventory_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="218">
   <si>
     <t>MedicineID</t>
   </si>
@@ -662,6 +662,18 @@
   </si>
   <si>
     <t>Drugs lol</t>
+  </si>
+  <si>
+    <t>DrugX</t>
+  </si>
+  <si>
+    <t>heart attacks</t>
+  </si>
+  <si>
+    <t>M102</t>
+  </si>
+  <si>
+    <t>heart attack</t>
   </si>
 </sst>
 </file>
@@ -3053,13 +3065,13 @@
         <v>17</v>
       </c>
       <c r="D101" s="2" t="n">
-        <v>43.0</v>
+        <v>25.0</v>
       </c>
       <c r="E101" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="2" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added default pwd feature and updated staff and inventory managers
</commit_message>
<xml_diff>
--- a/data/MedicalInventory_List.xlsx
+++ b/data/MedicalInventory_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="222">
   <si>
     <t>MedicineID</t>
   </si>
@@ -674,6 +674,18 @@
   </si>
   <si>
     <t>heart attack</t>
+  </si>
+  <si>
+    <t>Chicken Rice</t>
+  </si>
+  <si>
+    <t>Very good food, good for the soul</t>
+  </si>
+  <si>
+    <t>NasiLemak</t>
+  </si>
+  <si>
+    <t>COconut</t>
   </si>
 </sst>
 </file>
@@ -3024,8 +3036,8 @@
       <c r="C99" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D99" s="2">
-        <v>119</v>
+      <c r="D99" s="2" t="n">
+        <v>120.0</v>
       </c>
       <c r="E99" s="2" t="b">
         <v>0</v>
@@ -3044,8 +3056,8 @@
       <c r="C100" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D100" s="2">
-        <v>37</v>
+      <c r="D100" s="2" t="n">
+        <v>37.0</v>
       </c>
       <c r="E100" s="2" t="b">
         <v>1</v>
@@ -3065,13 +3077,13 @@
         <v>17</v>
       </c>
       <c r="D101" s="2" t="n">
-        <v>25.0</v>
+        <v>35.0</v>
       </c>
       <c r="E101" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F101" s="2" t="n">
-        <v>30.0</v>
+        <v>40.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>